<commit_message>
contribution sheet updated for week 2
</commit_message>
<xml_diff>
--- a/Contribution Spreadsheet SET09623 (Group 2).xlsx
+++ b/Contribution Spreadsheet SET09623 (Group 2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Dropbox\BSc (Hons)\DevOps\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3411A6C3-AC02-4F2C-B591-D74C10169370}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF48C715-595B-4DFB-8A80-F2905203EBD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C81EAE5-9AC4-4E43-98CD-A19758BE81E9}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{7C81EAE5-9AC4-4E43-98CD-A19758BE81E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,6 +475,9 @@
       <c r="C2" s="2">
         <v>25</v>
       </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -486,6 +489,9 @@
       <c r="C3" s="2">
         <v>25</v>
       </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -497,6 +503,9 @@
       <c r="C4" s="2">
         <v>25</v>
       </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -508,6 +517,9 @@
       <c r="C5" s="2">
         <v>25</v>
       </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -519,7 +531,7 @@
       </c>
       <c r="D7">
         <f>SUM(D2,D3,D4,D5)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <f>SUM(E2,E3,E4,E5)</f>

</xml_diff>

<commit_message>
Contribution spread sheet updated for week 3
</commit_message>
<xml_diff>
--- a/Contribution Spreadsheet SET09623 (Group 2).xlsx
+++ b/Contribution Spreadsheet SET09623 (Group 2).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Dropbox\BSc (Hons)\DevOps\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bsc (Hons)\DevOps\Coursework-group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF48C715-595B-4DFB-8A80-F2905203EBD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED62921-2A4C-4FD9-BBA9-40BE6044769E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{7C81EAE5-9AC4-4E43-98CD-A19758BE81E9}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,6 +478,9 @@
       <c r="D2">
         <v>25</v>
       </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -492,6 +495,9 @@
       <c r="D3">
         <v>25</v>
       </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -506,6 +512,9 @@
       <c r="D4">
         <v>25</v>
       </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -520,6 +529,9 @@
       <c r="D5">
         <v>25</v>
       </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -535,7 +547,7 @@
       </c>
       <c r="E7">
         <f>SUM(E2,E3,E4,E5)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <f>SUM(F2,F3,F4,F5)</f>

</xml_diff>